<commit_message>
Remove carriage returns from logistic phase description.
</commit_message>
<xml_diff>
--- a/dtocean_installation/config/operations_time_OLC.xlsx
+++ b/dtocean_installation/config/operations_time_OLC.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcvicente\Dropbox\DTocean\2. Working documents\WP5\DTOcean_WP5_dropbox\BitBucket_WavEC\examples\databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-installation\dtocean_installation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="operations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -474,20 +474,9 @@
     <t>Install_mattress</t>
   </si>
   <si>
-    <t>Lift and overboard concrete mattress +
-Lower concrete mattress to seabed +
-Position and release concrete mattress +
-Recover installation frame</t>
-  </si>
-  <si>
     <t>Install_rockbag</t>
   </si>
   <si>
-    <t>Lift and overboard rock filter bag +
-Lower rock filter bag to seabed +
-Position and release concrete mattress</t>
-  </si>
-  <si>
     <t>VessPrep_external</t>
   </si>
   <si>
@@ -549,6 +538,12 @@
   </si>
   <si>
     <t>VesPosCables</t>
+  </si>
+  <si>
+    <t>Lift and overboard rock filter bag + Lower rock filter bag to seabed + Position and release concrete mattress</t>
+  </si>
+  <si>
+    <t>Lift and overboard concrete mattress + Lower concrete mattress to seabed + Position and release concrete mattress + Recover installation frame</t>
   </si>
 </sst>
 </file>
@@ -1593,23 +1588,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1645,23 +1623,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1820,26 +1781,26 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125"/>
-    <col min="5" max="5" width="24.5703125"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125"/>
-    <col min="12" max="1025" width="8.5703125"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="53.7265625" customWidth="1"/>
+    <col min="4" max="4" width="21.453125"/>
+    <col min="5" max="5" width="24.54296875"/>
+    <col min="6" max="6" width="30.81640625" customWidth="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.453125" customWidth="1"/>
+    <col min="10" max="10" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.453125"/>
+    <col min="12" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="31"/>
       <c r="B1" s="26" t="s">
         <v>0</v>
@@ -1872,7 +1833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
@@ -1893,7 +1854,7 @@
       <c r="J2" s="38"/>
       <c r="K2" s="41"/>
     </row>
-    <row r="3" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="82" t="s">
         <v>12</v>
       </c>
@@ -1914,7 +1875,7 @@
       <c r="J3" s="85"/>
       <c r="K3" s="88"/>
     </row>
-    <row r="4" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="82" t="s">
         <v>14</v>
       </c>
@@ -1935,15 +1896,15 @@
       <c r="J4" s="85"/>
       <c r="K4" s="88"/>
     </row>
-    <row r="5" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5" s="18">
         <v>103</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D5" s="1">
         <v>12</v>
@@ -1956,15 +1917,15 @@
       <c r="J5" s="16"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="18">
         <v>104</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="1">
         <v>4</v>
@@ -1977,15 +1938,15 @@
       <c r="J6" s="16"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B7" s="18">
         <v>105</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -1998,15 +1959,15 @@
       <c r="J7" s="16"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B8" s="18">
         <v>106</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D8" s="1">
         <v>4</v>
@@ -2019,15 +1980,15 @@
       <c r="J8" s="16"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="18">
         <v>107</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
@@ -2040,15 +2001,15 @@
       <c r="J9" s="16"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B10" s="18">
         <v>108</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
@@ -2061,15 +2022,15 @@
       <c r="J10" s="16"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" s="18">
         <v>109</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D11" s="1">
         <v>12</v>
@@ -2082,15 +2043,15 @@
       <c r="J11" s="16"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" s="18">
         <v>110</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1">
         <v>48</v>
@@ -2103,15 +2064,15 @@
       <c r="J12" s="16"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" s="18">
         <v>111</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -2124,15 +2085,15 @@
       <c r="J13" s="16"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B14" s="18">
         <v>112</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D14" s="1">
         <v>4</v>
@@ -2145,7 +2106,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
         <v>16</v>
       </c>
@@ -2174,7 +2135,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
         <v>18</v>
       </c>
@@ -2203,7 +2164,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="33" t="s">
         <v>20</v>
       </c>
@@ -2232,7 +2193,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="33" t="s">
         <v>22</v>
       </c>
@@ -2253,7 +2214,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="82" t="s">
         <v>24</v>
       </c>
@@ -2282,7 +2243,7 @@
       </c>
       <c r="K19" s="88"/>
     </row>
-    <row r="20" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
@@ -2311,7 +2272,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="33" t="s">
         <v>28</v>
       </c>
@@ -2338,7 +2299,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="90" t="s">
         <v>109</v>
       </c>
@@ -2367,9 +2328,9 @@
       </c>
       <c r="K22" s="93"/>
     </row>
-    <row r="23" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="53" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B23" s="54">
         <v>121</v>
@@ -2396,7 +2357,7 @@
       </c>
       <c r="K23" s="57"/>
     </row>
-    <row r="24" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="53" t="s">
         <v>30</v>
       </c>
@@ -2425,7 +2386,7 @@
       </c>
       <c r="K24" s="67"/>
     </row>
-    <row r="25" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="62" t="s">
         <v>32</v>
       </c>
@@ -2446,7 +2407,7 @@
       <c r="J25" s="44"/>
       <c r="K25" s="45"/>
     </row>
-    <row r="26" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="63" t="s">
         <v>34</v>
       </c>
@@ -2475,7 +2436,7 @@
       </c>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="63" t="s">
         <v>36</v>
       </c>
@@ -2504,7 +2465,7 @@
       </c>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="63" t="s">
         <v>38</v>
       </c>
@@ -2533,7 +2494,7 @@
       </c>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="63" t="s">
         <v>40</v>
       </c>
@@ -2562,7 +2523,7 @@
       </c>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="63" t="s">
         <v>132</v>
       </c>
@@ -2591,7 +2552,7 @@
       </c>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="63" t="s">
         <v>128</v>
       </c>
@@ -2620,7 +2581,7 @@
       </c>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="63" t="s">
         <v>129</v>
       </c>
@@ -2649,7 +2610,7 @@
       </c>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="63" t="s">
         <v>130</v>
       </c>
@@ -2678,7 +2639,7 @@
       </c>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="63" t="s">
         <v>131</v>
       </c>
@@ -2707,7 +2668,7 @@
       </c>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="63" t="s">
         <v>121</v>
       </c>
@@ -2734,7 +2695,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="63" t="s">
         <v>126</v>
       </c>
@@ -2761,7 +2722,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="63" t="s">
         <v>120</v>
       </c>
@@ -2790,7 +2751,7 @@
       </c>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="63" t="s">
         <v>122</v>
       </c>
@@ -2819,7 +2780,7 @@
       </c>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="63" t="s">
         <v>125</v>
       </c>
@@ -2848,7 +2809,7 @@
       </c>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="63" t="s">
         <v>124</v>
       </c>
@@ -2877,7 +2838,7 @@
       </c>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="63" t="s">
         <v>123</v>
       </c>
@@ -2906,7 +2867,7 @@
       </c>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="63" t="s">
         <v>133</v>
       </c>
@@ -2935,7 +2896,7 @@
       </c>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="71" t="s">
         <v>118</v>
       </c>
@@ -2964,7 +2925,7 @@
       </c>
       <c r="K43" s="67"/>
     </row>
-    <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="71" t="s">
         <v>150</v>
       </c>
@@ -2972,7 +2933,7 @@
         <v>219</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="D44" s="3">
         <v>0.5</v>
@@ -2993,15 +2954,15 @@
       </c>
       <c r="K44" s="67"/>
     </row>
-    <row r="45" spans="1:11" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B45" s="78">
         <v>220</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="D45" s="42">
         <v>0.5</v>
@@ -3022,7 +2983,7 @@
       </c>
       <c r="K45" s="43"/>
     </row>
-    <row r="46" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="94" t="s">
         <v>103</v>
       </c>
@@ -3049,7 +3010,7 @@
       </c>
       <c r="K46" s="102"/>
     </row>
-    <row r="47" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="69" t="s">
         <v>102</v>
       </c>
@@ -3076,7 +3037,7 @@
       </c>
       <c r="K47" s="8"/>
     </row>
-    <row r="48" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="33" t="s">
         <v>53</v>
       </c>
@@ -3103,7 +3064,7 @@
       </c>
       <c r="K48" s="8"/>
     </row>
-    <row r="49" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="33" t="s">
         <v>55</v>
       </c>
@@ -3130,7 +3091,7 @@
       </c>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="33" t="s">
         <v>57</v>
       </c>
@@ -3157,7 +3118,7 @@
       </c>
       <c r="K50" s="8"/>
     </row>
-    <row r="51" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="33" t="s">
         <v>59</v>
       </c>
@@ -3178,7 +3139,7 @@
       <c r="J51" s="4"/>
       <c r="K51" s="8"/>
     </row>
-    <row r="52" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="34" t="s">
         <v>147</v>
       </c>
@@ -3205,7 +3166,7 @@
       </c>
       <c r="K52" s="51"/>
     </row>
-    <row r="53" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>60</v>
       </c>
@@ -3232,7 +3193,7 @@
       </c>
       <c r="K53" s="48"/>
     </row>
-    <row r="54" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="33" t="s">
         <v>95</v>
       </c>
@@ -3259,7 +3220,7 @@
       </c>
       <c r="K54" s="8"/>
     </row>
-    <row r="55" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="33" t="s">
         <v>94</v>
       </c>
@@ -3280,7 +3241,7 @@
       <c r="J55" s="4"/>
       <c r="K55" s="8"/>
     </row>
-    <row r="56" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="70" t="s">
         <v>61</v>
       </c>
@@ -3307,7 +3268,7 @@
       </c>
       <c r="K56" s="6"/>
     </row>
-    <row r="57" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="33" t="s">
         <v>62</v>
       </c>
@@ -3334,7 +3295,7 @@
       </c>
       <c r="K57" s="8"/>
     </row>
-    <row r="58" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="33" t="s">
         <v>63</v>
       </c>
@@ -3361,7 +3322,7 @@
       </c>
       <c r="K58" s="6"/>
     </row>
-    <row r="59" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="34" t="s">
         <v>64</v>
       </c>
@@ -3382,7 +3343,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="10"/>
     </row>
-    <row r="60" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="35" t="s">
         <v>66</v>
       </c>
@@ -3403,7 +3364,7 @@
       <c r="J60" s="22"/>
       <c r="K60" s="25"/>
     </row>
-    <row r="61" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="33" t="s">
         <v>68</v>
       </c>
@@ -3424,7 +3385,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="6"/>
     </row>
-    <row r="62" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="33" t="s">
         <v>70</v>
       </c>
@@ -3445,7 +3406,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="6"/>
     </row>
-    <row r="63" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="33" t="s">
         <v>72</v>
       </c>
@@ -3466,7 +3427,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="6"/>
     </row>
-    <row r="64" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="89" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="82" t="s">
         <v>74</v>
       </c>
@@ -3487,7 +3448,7 @@
       <c r="J64" s="85"/>
       <c r="K64" s="88"/>
     </row>
-    <row r="65" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="33" t="s">
         <v>76</v>
       </c>
@@ -3516,7 +3477,7 @@
       </c>
       <c r="K65" s="6"/>
     </row>
-    <row r="66" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="33" t="s">
         <v>78</v>
       </c>
@@ -3545,7 +3506,7 @@
       </c>
       <c r="K66" s="6"/>
     </row>
-    <row r="67" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="33" t="s">
         <v>80</v>
       </c>
@@ -3576,7 +3537,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="34" t="s">
         <v>83</v>
       </c>
@@ -3607,7 +3568,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="59" t="s">
         <v>107</v>
       </c>
@@ -3633,7 +3594,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="59" t="s">
         <v>110</v>
       </c>

</xml_diff>